<commit_message>
Add dismissible form messages and enhance error/success components
- Updated FormError and FormSuccess components to support dismissal
- Added resetSignal prop to trigger message re-display
- Implemented close button with Cross2Icon for each message
- Updated multiple pages to use new resetSignal functionality
- Improved user experience by allowing manual message dismissal
</commit_message>
<xml_diff>
--- a/public/workReportDefaultTemplate.xlsx
+++ b/public/workReportDefaultTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\furugakihiromitsu\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3E5779-A296-4EC8-A2DC-B8710994CED3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96F76F15-BA20-4814-91B0-D6EE4A604817}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="作業報告書" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">作業報告書!$A$1:$Y$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">作業報告書!$A$1:$V$49</definedName>
     <definedName name="タイトル">作業報告書!$A$1</definedName>
     <definedName name="稼働時間">作業報告書!$J$14:$K$44</definedName>
     <definedName name="開始時刻">作業報告書!$D$14:$E$44</definedName>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>祝日</t>
   </si>
@@ -71,12 +71,6 @@
   </si>
   <si>
     <t>氏名：</t>
-  </si>
-  <si>
-    <t>本人印</t>
-  </si>
-  <si>
-    <t>承認印</t>
   </si>
   <si>
     <t>日付</t>
@@ -899,7 +893,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="135">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -999,44 +993,58 @@
     <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="56" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
+    <xf numFmtId="181" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -1050,63 +1058,159 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="56" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="56" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="180" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="180" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
@@ -1123,34 +1227,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="180" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="180" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1199,139 +1275,78 @@
     <xf numFmtId="0" fontId="9" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="181" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="56" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="6" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="179" fontId="6" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1395,61 +1410,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>27214</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>40821</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>367392</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>204106</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="図 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B31EA252-9F9E-71F5-25CA-D2D5202DDA96}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8313964" y="1183821"/>
-          <a:ext cx="734785" cy="734785"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1772,14 +1732,14 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="34"/>
-      <c r="D1" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="34"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="35"/>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
@@ -1802,11 +1762,11 @@
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E2" s="4"/>
       <c r="F2" s="7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
@@ -1831,7 +1791,7 @@
         <v>45709</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E3" s="4">
         <v>6.9444400000000001E-4</v>
@@ -1862,7 +1822,7 @@
         <v>45737</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E4" s="4">
         <v>3.4722220000000001E-3</v>
@@ -1893,13 +1853,13 @@
         <v>45768</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="4">
         <v>6.9444440000000001E-3</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -1924,13 +1884,13 @@
         <v>45798</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E6" s="4">
         <v>1.0416666E-2</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
@@ -1955,13 +1915,13 @@
         <v>45829</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="4">
         <v>2.0833332999999999E-2</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
@@ -1980,7 +1940,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="4">
         <v>4.1666665999999998E-2</v>
@@ -18950,11 +18910,11 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC49"/>
+  <dimension ref="A1:AC50"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="13" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R4" sqref="R4:T5"/>
+      <selection pane="bottomLeft" sqref="A1:J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -18968,66 +18928,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="23.1" customHeight="1">
-      <c r="A1" s="63"/>
-      <c r="B1" s="64"/>
-      <c r="C1" s="64"/>
-      <c r="D1" s="64"/>
-      <c r="E1" s="64"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="64"/>
-      <c r="H1" s="64"/>
-      <c r="I1" s="64"/>
-      <c r="J1" s="64"/>
+      <c r="A1" s="99"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
       <c r="K1" s="10"/>
       <c r="L1" s="11"/>
       <c r="M1" s="11"/>
       <c r="N1" s="11"/>
       <c r="O1" s="11"/>
       <c r="P1" s="11"/>
-      <c r="Q1" s="66" t="s">
+      <c r="Q1" s="102" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="67"/>
-      <c r="S1" s="69" t="s">
-        <v>54</v>
-      </c>
-      <c r="T1" s="70"/>
-      <c r="U1" s="70"/>
-      <c r="V1" s="70"/>
-      <c r="W1" s="70"/>
-      <c r="X1" s="70"/>
-      <c r="Y1" s="70"/>
+      <c r="R1" s="103"/>
+      <c r="S1" s="125" t="s">
+        <v>52</v>
+      </c>
+      <c r="T1" s="125"/>
+      <c r="U1" s="125"/>
+      <c r="V1" s="125"/>
+      <c r="W1" s="124"/>
+      <c r="X1" s="124"/>
+      <c r="Y1" s="124"/>
       <c r="Z1" s="12"/>
       <c r="AA1" s="11"/>
     </row>
     <row r="2" spans="1:29" ht="23.1" customHeight="1" thickBot="1">
-      <c r="A2" s="65"/>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
+      <c r="A2" s="101"/>
+      <c r="B2" s="101"/>
+      <c r="C2" s="101"/>
+      <c r="D2" s="101"/>
+      <c r="E2" s="101"/>
+      <c r="F2" s="101"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
+      <c r="J2" s="101"/>
       <c r="K2" s="14"/>
       <c r="L2" s="15"/>
       <c r="M2" s="15"/>
       <c r="N2" s="15"/>
       <c r="O2" s="15"/>
       <c r="P2" s="15"/>
-      <c r="Q2" s="68"/>
-      <c r="R2" s="68"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="65"/>
-      <c r="X2" s="65"/>
-      <c r="Y2" s="65"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="11"/>
+      <c r="Q2" s="104"/>
+      <c r="R2" s="104"/>
+      <c r="S2" s="126"/>
+      <c r="T2" s="126"/>
+      <c r="U2" s="126"/>
+      <c r="V2" s="126"/>
+      <c r="W2" s="136"/>
+      <c r="X2" s="136"/>
+      <c r="Y2" s="136"/>
+      <c r="Z2" s="137"/>
+      <c r="AA2" s="138"/>
+      <c r="AB2" s="139"/>
     </row>
     <row r="3" spans="1:29" ht="23.1" customHeight="1">
       <c r="A3" s="16" t="str">
@@ -19061,144 +19022,140 @@
       <c r="Z3" s="17"/>
       <c r="AA3" s="18"/>
       <c r="AC3" s="26" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="23.1" customHeight="1" outlineLevel="1">
-      <c r="A4" s="71" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="72"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="74">
+      <c r="A4" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="78">
         <v>0.375</v>
       </c>
-      <c r="F4" s="75"/>
-      <c r="G4" s="76"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="79"/>
       <c r="H4" s="28"/>
-      <c r="I4" s="77" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="78"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="86">
+      <c r="I4" s="105" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="106"/>
+      <c r="K4" s="107"/>
+      <c r="L4" s="114">
         <f>COUNT(稼働時間, "&gt;0")</f>
         <v>0</v>
       </c>
-      <c r="M4" s="87"/>
-      <c r="O4" s="88" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="90"/>
-      <c r="R4" s="80">
+      <c r="M4" s="115"/>
+      <c r="O4" s="116" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" s="117"/>
+      <c r="Q4" s="118"/>
+      <c r="R4" s="108">
         <f>SUM(稼働時間)</f>
         <v>0</v>
       </c>
-      <c r="S4" s="81"/>
-      <c r="T4" s="82"/>
+      <c r="S4" s="109"/>
+      <c r="T4" s="110"/>
       <c r="U4" s="17"/>
-      <c r="V4" s="55" t="s">
-        <v>8</v>
-      </c>
-      <c r="W4" s="56"/>
-      <c r="X4" s="55" t="s">
-        <v>9</v>
-      </c>
-      <c r="Y4" s="56"/>
+      <c r="V4" s="141"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="72"/>
+      <c r="Y4" s="73"/>
       <c r="AB4" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="AC4" s="25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="23.1" customHeight="1" outlineLevel="1">
-      <c r="A5" s="71" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="74">
+      <c r="A5" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="78">
         <v>0.75</v>
       </c>
-      <c r="F5" s="75"/>
-      <c r="G5" s="76"/>
+      <c r="F5" s="78"/>
+      <c r="G5" s="79"/>
       <c r="H5" s="30"/>
-      <c r="O5" s="91"/>
-      <c r="P5" s="77"/>
-      <c r="Q5" s="92"/>
-      <c r="R5" s="83"/>
-      <c r="S5" s="84"/>
-      <c r="T5" s="85"/>
+      <c r="O5" s="119"/>
+      <c r="P5" s="105"/>
+      <c r="Q5" s="120"/>
+      <c r="R5" s="111"/>
+      <c r="S5" s="112"/>
+      <c r="T5" s="113"/>
       <c r="U5" s="17"/>
-      <c r="V5" s="57"/>
-      <c r="W5" s="58"/>
-      <c r="X5" s="57"/>
-      <c r="Y5" s="58"/>
+      <c r="V5" s="140"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="74"/>
+      <c r="Y5" s="75"/>
       <c r="AB5" s="24" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="AC5" s="25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="23.1" customHeight="1" outlineLevel="1">
-      <c r="A6" s="71" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="72"/>
-      <c r="C6" s="72"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="74">
+      <c r="A6" s="52" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="77">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="F6" s="75"/>
-      <c r="G6" s="76"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="79"/>
       <c r="H6" s="30"/>
-      <c r="I6" s="93"/>
-      <c r="J6" s="93"/>
-      <c r="K6" s="93"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="94"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="76"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
       <c r="O6" s="22"/>
       <c r="Q6" s="22"/>
       <c r="R6" s="32"/>
       <c r="S6" s="31"/>
       <c r="T6" s="31"/>
       <c r="U6" s="17"/>
-      <c r="V6" s="59"/>
-      <c r="W6" s="60"/>
-      <c r="X6" s="59"/>
-      <c r="Y6" s="60"/>
+      <c r="V6" s="33"/>
+      <c r="W6" s="33"/>
+      <c r="X6" s="75"/>
+      <c r="Y6" s="75"/>
       <c r="AB6" s="24" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="AC6" s="25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="23.1" customHeight="1" outlineLevel="1">
-      <c r="A7" s="71" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="72"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="107">
+      <c r="A7" s="52" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="55">
         <f>IF(E5="","",E5-E4-E6)</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F7" s="108"/>
-      <c r="G7" s="109"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="57"/>
       <c r="H7" s="30"/>
-      <c r="I7" s="93"/>
-      <c r="J7" s="93"/>
-      <c r="K7" s="93"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="94"/>
+      <c r="I7" s="76"/>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
       <c r="O7" s="22"/>
       <c r="P7" s="22"/>
       <c r="Q7" s="22"/>
@@ -19206,50 +19163,50 @@
       <c r="S7" s="31"/>
       <c r="T7" s="31"/>
       <c r="U7" s="17"/>
-      <c r="V7" s="61"/>
-      <c r="W7" s="62"/>
-      <c r="X7" s="61"/>
-      <c r="Y7" s="62"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="33"/>
+      <c r="X7" s="75"/>
+      <c r="Y7" s="75"/>
       <c r="AB7" s="24" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AC7" s="25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="23.1" customHeight="1" outlineLevel="1">
-      <c r="A8" s="110" t="s">
-        <v>23</v>
-      </c>
-      <c r="B8" s="72"/>
-      <c r="C8" s="72"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="111" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="112"/>
-      <c r="G8" s="113"/>
+      <c r="A8" s="58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="60"/>
+      <c r="G8" s="61"/>
       <c r="H8" s="17"/>
       <c r="U8" s="17"/>
       <c r="AB8" s="24" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="AC8" s="25" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="23.1" customHeight="1" outlineLevel="1">
-      <c r="A9" s="110" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="72"/>
-      <c r="D9" s="72"/>
-      <c r="E9" s="111" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="112"/>
-      <c r="G9" s="113"/>
+      <c r="A9" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="53"/>
+      <c r="C9" s="53"/>
+      <c r="D9" s="53"/>
+      <c r="E9" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="60"/>
+      <c r="G9" s="61"/>
       <c r="H9" s="17"/>
       <c r="O9" s="17"/>
       <c r="U9" s="17"/>
@@ -19259,10 +19216,10 @@
       <c r="Y9" s="17"/>
       <c r="AA9" s="19"/>
       <c r="AB9" s="24" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="AC9" s="25" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="23.1" customHeight="1" outlineLevel="1">
@@ -19294,1208 +19251,1208 @@
       <c r="Z10" s="17"/>
       <c r="AA10" s="18"/>
       <c r="AB10" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC10" s="25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" ht="23.1" customHeight="1">
+      <c r="A11" s="62" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="63"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="AC10" s="25" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:29" ht="23.1" customHeight="1">
-      <c r="A11" s="95" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="114"/>
-      <c r="C11" s="115"/>
-      <c r="D11" s="95" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="96"/>
-      <c r="F11" s="95" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="96"/>
-      <c r="H11" s="95" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="96"/>
-      <c r="J11" s="99" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11" s="100"/>
-      <c r="L11" s="99" t="s">
-        <v>55</v>
-      </c>
-      <c r="M11" s="105"/>
-      <c r="N11" s="105"/>
-      <c r="O11" s="105"/>
-      <c r="P11" s="105"/>
-      <c r="Q11" s="105"/>
-      <c r="R11" s="105"/>
-      <c r="S11" s="105"/>
-      <c r="T11" s="105"/>
-      <c r="U11" s="105"/>
-      <c r="V11" s="100"/>
+      <c r="E11" s="90"/>
+      <c r="F11" s="62" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="90"/>
+      <c r="H11" s="62" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="90"/>
+      <c r="J11" s="93" t="s">
+        <v>25</v>
+      </c>
+      <c r="K11" s="94"/>
+      <c r="L11" s="93" t="s">
+        <v>53</v>
+      </c>
+      <c r="M11" s="97"/>
+      <c r="N11" s="97"/>
+      <c r="O11" s="97"/>
+      <c r="P11" s="97"/>
+      <c r="Q11" s="97"/>
+      <c r="R11" s="97"/>
+      <c r="S11" s="97"/>
+      <c r="T11" s="97"/>
+      <c r="U11" s="97"/>
+      <c r="V11" s="94"/>
       <c r="W11" s="24"/>
       <c r="AB11" s="13"/>
       <c r="AC11" s="25" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:29" ht="23.1" customHeight="1">
-      <c r="A12" s="116"/>
-      <c r="B12" s="117"/>
-      <c r="C12" s="118"/>
-      <c r="D12" s="97"/>
-      <c r="E12" s="98"/>
-      <c r="F12" s="97"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="97"/>
-      <c r="I12" s="98"/>
-      <c r="J12" s="101"/>
-      <c r="K12" s="102"/>
-      <c r="L12" s="101"/>
-      <c r="M12" s="106"/>
-      <c r="N12" s="106"/>
-      <c r="O12" s="106"/>
-      <c r="P12" s="106"/>
-      <c r="Q12" s="106"/>
-      <c r="R12" s="106"/>
-      <c r="S12" s="106"/>
-      <c r="T12" s="106"/>
-      <c r="U12" s="106"/>
-      <c r="V12" s="102"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="66"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="91"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="91"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="95"/>
+      <c r="K12" s="96"/>
+      <c r="L12" s="95"/>
+      <c r="M12" s="98"/>
+      <c r="N12" s="98"/>
+      <c r="O12" s="98"/>
+      <c r="P12" s="98"/>
+      <c r="Q12" s="98"/>
+      <c r="R12" s="98"/>
+      <c r="S12" s="98"/>
+      <c r="T12" s="98"/>
+      <c r="U12" s="98"/>
+      <c r="V12" s="96"/>
       <c r="AB12" s="24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="AC12" s="25" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:29" ht="23.1" customHeight="1" thickBot="1">
-      <c r="A13" s="119" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="120"/>
-      <c r="C13" s="120"/>
-      <c r="D13" s="121">
+      <c r="A13" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="47">
         <v>0.41666666666666669</v>
       </c>
-      <c r="E13" s="122"/>
-      <c r="F13" s="121">
+      <c r="E13" s="48"/>
+      <c r="F13" s="47">
         <v>0.79166666666666663</v>
       </c>
-      <c r="G13" s="122"/>
-      <c r="H13" s="123">
+      <c r="G13" s="48"/>
+      <c r="H13" s="45">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="I13" s="124"/>
-      <c r="J13" s="121">
+      <c r="I13" s="46"/>
+      <c r="J13" s="47">
         <v>0.33333333333333331</v>
       </c>
-      <c r="K13" s="122"/>
-      <c r="L13" s="129" t="s">
-        <v>29</v>
-      </c>
-      <c r="M13" s="130"/>
-      <c r="N13" s="130"/>
-      <c r="O13" s="130"/>
-      <c r="P13" s="130"/>
-      <c r="Q13" s="130"/>
-      <c r="R13" s="130"/>
-      <c r="S13" s="130"/>
-      <c r="T13" s="130"/>
-      <c r="U13" s="130"/>
-      <c r="V13" s="131"/>
+      <c r="K13" s="48"/>
+      <c r="L13" s="84" t="s">
+        <v>27</v>
+      </c>
+      <c r="M13" s="85"/>
+      <c r="N13" s="85"/>
+      <c r="O13" s="85"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="85"/>
+      <c r="R13" s="85"/>
+      <c r="S13" s="85"/>
+      <c r="T13" s="85"/>
+      <c r="U13" s="85"/>
+      <c r="V13" s="86"/>
       <c r="W13" s="24"/>
       <c r="X13" s="25"/>
       <c r="AB13" s="13"/>
     </row>
     <row r="14" spans="1:29" ht="23.1" customHeight="1">
-      <c r="A14" s="103" t="str">
+      <c r="A14" s="70" t="str">
         <f ca="1">IFERROR(VLOOKUP(A1,マスタ!$B$3:$C$7,2,0),"")</f>
         <v/>
       </c>
-      <c r="B14" s="104"/>
+      <c r="B14" s="71"/>
       <c r="C14" s="20" t="str">
         <f ca="1">IF(A14="","", TEXT(A14,"aaa"))</f>
         <v/>
       </c>
-      <c r="D14" s="51"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="49"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="125"/>
-      <c r="I14" s="126"/>
-      <c r="J14" s="127" t="str">
+      <c r="D14" s="42"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="37"/>
+      <c r="H14" s="80"/>
+      <c r="I14" s="81"/>
+      <c r="J14" s="82" t="str">
         <f t="shared" ref="J14" si="0">IF(D14="","",(ABS(F14-D14))-H14)</f>
         <v/>
       </c>
-      <c r="K14" s="128"/>
-      <c r="L14" s="132"/>
-      <c r="M14" s="133"/>
-      <c r="N14" s="133"/>
-      <c r="O14" s="133"/>
-      <c r="P14" s="133"/>
-      <c r="Q14" s="133"/>
-      <c r="R14" s="133"/>
-      <c r="S14" s="133"/>
-      <c r="T14" s="133"/>
-      <c r="U14" s="133"/>
-      <c r="V14" s="134"/>
+      <c r="K14" s="83"/>
+      <c r="L14" s="87"/>
+      <c r="M14" s="88"/>
+      <c r="N14" s="88"/>
+      <c r="O14" s="88"/>
+      <c r="P14" s="88"/>
+      <c r="Q14" s="88"/>
+      <c r="R14" s="88"/>
+      <c r="S14" s="88"/>
+      <c r="T14" s="88"/>
+      <c r="U14" s="88"/>
+      <c r="V14" s="89"/>
       <c r="W14" s="23"/>
       <c r="AB14" s="13"/>
     </row>
     <row r="15" spans="1:29" ht="23.1" customHeight="1">
-      <c r="A15" s="47" t="str">
+      <c r="A15" s="40" t="str">
         <f ca="1">IF(A14="","",
 IF(OR(DAY(A14+1)&lt;=20, MONTH($A$14)=MONTH(A14+1)),A14+1,""))</f>
         <v/>
       </c>
-      <c r="B15" s="48"/>
+      <c r="B15" s="41"/>
       <c r="C15" s="21" t="str">
         <f t="shared" ref="C15:C44" ca="1" si="1">IF(A15="","", TEXT(A15,"aaa"))</f>
         <v/>
       </c>
-      <c r="D15" s="51"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="49"/>
-      <c r="G15" s="50"/>
-      <c r="H15" s="49"/>
-      <c r="I15" s="50"/>
-      <c r="J15" s="53" t="str">
+      <c r="D15" s="42"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="36"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="36"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="38" t="str">
         <f t="shared" ref="J15:J44" si="2">IF(D15="","",(ABS(F15-D15))-H15)</f>
         <v/>
       </c>
-      <c r="K15" s="54"/>
-      <c r="L15" s="44"/>
-      <c r="M15" s="45"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="45"/>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="45"/>
-      <c r="S15" s="45"/>
-      <c r="T15" s="45"/>
-      <c r="U15" s="45"/>
-      <c r="V15" s="46"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="49"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="50"/>
+      <c r="Q15" s="50"/>
+      <c r="R15" s="50"/>
+      <c r="S15" s="50"/>
+      <c r="T15" s="50"/>
+      <c r="U15" s="50"/>
+      <c r="V15" s="51"/>
       <c r="W15" s="23"/>
       <c r="AB15" s="13"/>
     </row>
     <row r="16" spans="1:29" ht="23.1" customHeight="1">
-      <c r="A16" s="47" t="str">
+      <c r="A16" s="40" t="str">
         <f t="shared" ref="A16:A23" ca="1" si="3">IF(A15="","",
 IF(OR(DAY(A15+1)&lt;=20, MONTH($A$14)=MONTH(A15+1)),A15+1,""))</f>
         <v/>
       </c>
-      <c r="B16" s="48"/>
+      <c r="B16" s="41"/>
       <c r="C16" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D16" s="51"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="49"/>
-      <c r="I16" s="50"/>
-      <c r="J16" s="53" t="str">
+      <c r="D16" s="42"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K16" s="54"/>
-      <c r="L16" s="44"/>
-      <c r="M16" s="45"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="45"/>
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="46"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="49"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="50"/>
+      <c r="P16" s="50"/>
+      <c r="Q16" s="50"/>
+      <c r="R16" s="50"/>
+      <c r="S16" s="50"/>
+      <c r="T16" s="50"/>
+      <c r="U16" s="50"/>
+      <c r="V16" s="51"/>
       <c r="W16" s="23"/>
       <c r="AB16" s="13"/>
     </row>
     <row r="17" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A17" s="47" t="str">
+      <c r="A17" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="B17" s="48"/>
+      <c r="B17" s="41"/>
       <c r="C17" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D17" s="51"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="52"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="53" t="str">
+      <c r="D17" s="42"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K17" s="54"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="45"/>
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45"/>
-      <c r="T17" s="45"/>
-      <c r="U17" s="45"/>
-      <c r="V17" s="46"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="49"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="50"/>
+      <c r="P17" s="50"/>
+      <c r="Q17" s="50"/>
+      <c r="R17" s="50"/>
+      <c r="S17" s="50"/>
+      <c r="T17" s="50"/>
+      <c r="U17" s="50"/>
+      <c r="V17" s="51"/>
       <c r="W17" s="23"/>
       <c r="AB17" s="13"/>
     </row>
     <row r="18" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A18" s="47" t="str">
+      <c r="A18" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="B18" s="48"/>
+      <c r="B18" s="41"/>
       <c r="C18" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D18" s="51"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="53" t="str">
+      <c r="D18" s="42"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="36"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K18" s="54"/>
-      <c r="L18" s="44"/>
-      <c r="M18" s="45"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="45"/>
-      <c r="P18" s="45"/>
-      <c r="Q18" s="45"/>
-      <c r="R18" s="45"/>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-      <c r="U18" s="45"/>
-      <c r="V18" s="46"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="49"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="50"/>
+      <c r="P18" s="50"/>
+      <c r="Q18" s="50"/>
+      <c r="R18" s="50"/>
+      <c r="S18" s="50"/>
+      <c r="T18" s="50"/>
+      <c r="U18" s="50"/>
+      <c r="V18" s="51"/>
       <c r="W18" s="23"/>
       <c r="AB18" s="13"/>
     </row>
     <row r="19" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A19" s="47" t="str">
+      <c r="A19" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="B19" s="48"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D19" s="51"/>
-      <c r="E19" s="52"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="50"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="53" t="str">
+      <c r="D19" s="42"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="37"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K19" s="54"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="45"/>
-      <c r="P19" s="45"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="45"/>
-      <c r="S19" s="45"/>
-      <c r="T19" s="45"/>
-      <c r="U19" s="45"/>
-      <c r="V19" s="46"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="50"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="50"/>
+      <c r="S19" s="50"/>
+      <c r="T19" s="50"/>
+      <c r="U19" s="50"/>
+      <c r="V19" s="51"/>
       <c r="W19" s="23"/>
       <c r="AB19" s="13"/>
     </row>
     <row r="20" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A20" s="47" t="str">
+      <c r="A20" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="B20" s="48"/>
+      <c r="B20" s="41"/>
       <c r="C20" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D20" s="51"/>
-      <c r="E20" s="52"/>
-      <c r="F20" s="49"/>
-      <c r="G20" s="50"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="53" t="str">
+      <c r="D20" s="42"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="37"/>
+      <c r="H20" s="36"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K20" s="54"/>
-      <c r="L20" s="44"/>
-      <c r="M20" s="45"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="45"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="45"/>
-      <c r="R20" s="45"/>
-      <c r="S20" s="45"/>
-      <c r="T20" s="45"/>
-      <c r="U20" s="45"/>
-      <c r="V20" s="46"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="49"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="50"/>
+      <c r="P20" s="50"/>
+      <c r="Q20" s="50"/>
+      <c r="R20" s="50"/>
+      <c r="S20" s="50"/>
+      <c r="T20" s="50"/>
+      <c r="U20" s="50"/>
+      <c r="V20" s="51"/>
       <c r="W20" s="23"/>
       <c r="AB20" s="13"/>
     </row>
     <row r="21" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A21" s="47" t="str">
+      <c r="A21" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="B21" s="48"/>
+      <c r="B21" s="41"/>
       <c r="C21" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D21" s="51"/>
-      <c r="E21" s="52"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="50"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="50"/>
-      <c r="J21" s="53" t="str">
+      <c r="D21" s="42"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="37"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K21" s="54"/>
-      <c r="L21" s="44"/>
-      <c r="M21" s="45"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="45"/>
-      <c r="P21" s="45"/>
-      <c r="Q21" s="45"/>
-      <c r="R21" s="45"/>
-      <c r="S21" s="45"/>
-      <c r="T21" s="45"/>
-      <c r="U21" s="45"/>
-      <c r="V21" s="46"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="50"/>
+      <c r="Q21" s="50"/>
+      <c r="R21" s="50"/>
+      <c r="S21" s="50"/>
+      <c r="T21" s="50"/>
+      <c r="U21" s="50"/>
+      <c r="V21" s="51"/>
       <c r="W21" s="23"/>
       <c r="AB21" s="13"/>
     </row>
     <row r="22" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A22" s="47" t="str">
+      <c r="A22" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="B22" s="48"/>
+      <c r="B22" s="41"/>
       <c r="C22" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D22" s="51"/>
-      <c r="E22" s="52"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="50"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="50"/>
-      <c r="J22" s="53" t="str">
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="36"/>
+      <c r="G22" s="37"/>
+      <c r="H22" s="36"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K22" s="54"/>
-      <c r="L22" s="44"/>
-      <c r="M22" s="45"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="45"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="45"/>
-      <c r="S22" s="45"/>
-      <c r="T22" s="45"/>
-      <c r="U22" s="45"/>
-      <c r="V22" s="46"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="49"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="50"/>
+      <c r="P22" s="50"/>
+      <c r="Q22" s="50"/>
+      <c r="R22" s="50"/>
+      <c r="S22" s="50"/>
+      <c r="T22" s="50"/>
+      <c r="U22" s="50"/>
+      <c r="V22" s="51"/>
       <c r="W22" s="23"/>
       <c r="AB22" s="13"/>
     </row>
     <row r="23" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A23" s="47" t="str">
+      <c r="A23" s="40" t="str">
         <f t="shared" ca="1" si="3"/>
         <v/>
       </c>
-      <c r="B23" s="48"/>
+      <c r="B23" s="41"/>
       <c r="C23" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D23" s="51"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="49"/>
-      <c r="G23" s="50"/>
-      <c r="H23" s="49"/>
-      <c r="I23" s="50"/>
-      <c r="J23" s="53" t="str">
+      <c r="D23" s="42"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="36"/>
+      <c r="G23" s="37"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K23" s="54"/>
-      <c r="L23" s="44"/>
-      <c r="M23" s="45"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="45"/>
-      <c r="P23" s="45"/>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="45"/>
-      <c r="S23" s="45"/>
-      <c r="T23" s="45"/>
-      <c r="U23" s="45"/>
-      <c r="V23" s="46"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="50"/>
+      <c r="Q23" s="50"/>
+      <c r="R23" s="50"/>
+      <c r="S23" s="50"/>
+      <c r="T23" s="50"/>
+      <c r="U23" s="50"/>
+      <c r="V23" s="51"/>
       <c r="W23" s="23"/>
       <c r="AB23" s="13"/>
     </row>
     <row r="24" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A24" s="47" t="str">
+      <c r="A24" s="40" t="str">
         <f t="shared" ref="A24:A35" ca="1" si="4">IF(A23="","",
 IF(OR(DAY(A23+1)&lt;=20, MONTH($A$14)=MONTH(A23+1)),A23+1,""))</f>
         <v/>
       </c>
-      <c r="B24" s="48"/>
+      <c r="B24" s="41"/>
       <c r="C24" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D24" s="49"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="49"/>
-      <c r="G24" s="50"/>
-      <c r="H24" s="49"/>
-      <c r="I24" s="50"/>
-      <c r="J24" s="53" t="str">
+      <c r="D24" s="36"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="37"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="37"/>
+      <c r="J24" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K24" s="54"/>
-      <c r="L24" s="44"/>
-      <c r="M24" s="45"/>
-      <c r="N24" s="45"/>
-      <c r="O24" s="45"/>
-      <c r="P24" s="45"/>
-      <c r="Q24" s="45"/>
-      <c r="R24" s="45"/>
-      <c r="S24" s="45"/>
-      <c r="T24" s="45"/>
-      <c r="U24" s="45"/>
-      <c r="V24" s="46"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="50"/>
+      <c r="Q24" s="50"/>
+      <c r="R24" s="50"/>
+      <c r="S24" s="50"/>
+      <c r="T24" s="50"/>
+      <c r="U24" s="50"/>
+      <c r="V24" s="51"/>
       <c r="W24" s="23"/>
       <c r="AB24" s="13"/>
     </row>
     <row r="25" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A25" s="47" t="str">
+      <c r="A25" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="B25" s="48"/>
+      <c r="B25" s="41"/>
       <c r="C25" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D25" s="49"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="49"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="49"/>
-      <c r="I25" s="50"/>
-      <c r="J25" s="53" t="str">
+      <c r="D25" s="36"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="37"/>
+      <c r="H25" s="36"/>
+      <c r="I25" s="37"/>
+      <c r="J25" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K25" s="54"/>
-      <c r="L25" s="44"/>
-      <c r="M25" s="45"/>
-      <c r="N25" s="45"/>
-      <c r="O25" s="45"/>
-      <c r="P25" s="45"/>
-      <c r="Q25" s="45"/>
-      <c r="R25" s="45"/>
-      <c r="S25" s="45"/>
-      <c r="T25" s="45"/>
-      <c r="U25" s="45"/>
-      <c r="V25" s="46"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="49"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="50"/>
+      <c r="P25" s="50"/>
+      <c r="Q25" s="50"/>
+      <c r="R25" s="50"/>
+      <c r="S25" s="50"/>
+      <c r="T25" s="50"/>
+      <c r="U25" s="50"/>
+      <c r="V25" s="51"/>
       <c r="W25" s="23"/>
       <c r="AB25" s="13"/>
     </row>
     <row r="26" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A26" s="47" t="str">
+      <c r="A26" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="B26" s="48"/>
+      <c r="B26" s="41"/>
       <c r="C26" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D26" s="51"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="49"/>
-      <c r="G26" s="50"/>
-      <c r="H26" s="49"/>
-      <c r="I26" s="50"/>
-      <c r="J26" s="53" t="str">
+      <c r="D26" s="42"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K26" s="54"/>
-      <c r="L26" s="44"/>
-      <c r="M26" s="45"/>
-      <c r="N26" s="45"/>
-      <c r="O26" s="45"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="45"/>
-      <c r="S26" s="45"/>
-      <c r="T26" s="45"/>
-      <c r="U26" s="45"/>
-      <c r="V26" s="46"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="50"/>
+      <c r="Q26" s="50"/>
+      <c r="R26" s="50"/>
+      <c r="S26" s="50"/>
+      <c r="T26" s="50"/>
+      <c r="U26" s="50"/>
+      <c r="V26" s="51"/>
       <c r="W26" s="23"/>
       <c r="AB26" s="13"/>
     </row>
     <row r="27" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A27" s="47" t="str">
+      <c r="A27" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="B27" s="48"/>
+      <c r="B27" s="41"/>
       <c r="C27" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D27" s="51"/>
-      <c r="E27" s="52"/>
-      <c r="F27" s="49"/>
-      <c r="G27" s="50"/>
-      <c r="H27" s="49"/>
-      <c r="I27" s="50"/>
-      <c r="J27" s="53" t="str">
+      <c r="D27" s="42"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="37"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="37"/>
+      <c r="J27" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K27" s="54"/>
-      <c r="L27" s="44"/>
-      <c r="M27" s="45"/>
-      <c r="N27" s="45"/>
-      <c r="O27" s="45"/>
-      <c r="P27" s="45"/>
-      <c r="Q27" s="45"/>
-      <c r="R27" s="45"/>
-      <c r="S27" s="45"/>
-      <c r="T27" s="45"/>
-      <c r="U27" s="45"/>
-      <c r="V27" s="46"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="50"/>
+      <c r="Q27" s="50"/>
+      <c r="R27" s="50"/>
+      <c r="S27" s="50"/>
+      <c r="T27" s="50"/>
+      <c r="U27" s="50"/>
+      <c r="V27" s="51"/>
       <c r="W27" s="23"/>
       <c r="AB27" s="13"/>
     </row>
     <row r="28" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A28" s="47" t="str">
+      <c r="A28" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="B28" s="48"/>
+      <c r="B28" s="41"/>
       <c r="C28" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D28" s="51"/>
-      <c r="E28" s="52"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="50"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="50"/>
-      <c r="J28" s="53" t="str">
+      <c r="D28" s="42"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K28" s="54"/>
-      <c r="L28" s="44"/>
-      <c r="M28" s="45"/>
-      <c r="N28" s="45"/>
-      <c r="O28" s="45"/>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="45"/>
-      <c r="U28" s="45"/>
-      <c r="V28" s="46"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="50"/>
+      <c r="Q28" s="50"/>
+      <c r="R28" s="50"/>
+      <c r="S28" s="50"/>
+      <c r="T28" s="50"/>
+      <c r="U28" s="50"/>
+      <c r="V28" s="51"/>
       <c r="W28" s="23"/>
       <c r="AB28" s="13"/>
     </row>
     <row r="29" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A29" s="47" t="str">
+      <c r="A29" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="B29" s="48"/>
+      <c r="B29" s="41"/>
       <c r="C29" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D29" s="51"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="49"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="53" t="str">
+      <c r="D29" s="42"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="36"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K29" s="54"/>
-      <c r="L29" s="44"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="45"/>
-      <c r="O29" s="45"/>
-      <c r="P29" s="45"/>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45"/>
-      <c r="T29" s="45"/>
-      <c r="U29" s="45"/>
-      <c r="V29" s="46"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="50"/>
+      <c r="Q29" s="50"/>
+      <c r="R29" s="50"/>
+      <c r="S29" s="50"/>
+      <c r="T29" s="50"/>
+      <c r="U29" s="50"/>
+      <c r="V29" s="51"/>
       <c r="W29" s="23"/>
       <c r="AB29" s="13"/>
     </row>
     <row r="30" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A30" s="47" t="str">
+      <c r="A30" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="B30" s="48"/>
+      <c r="B30" s="41"/>
       <c r="C30" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D30" s="51"/>
-      <c r="E30" s="52"/>
-      <c r="F30" s="49"/>
-      <c r="G30" s="50"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="50"/>
-      <c r="J30" s="53" t="str">
+      <c r="D30" s="42"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="37"/>
+      <c r="H30" s="36"/>
+      <c r="I30" s="37"/>
+      <c r="J30" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K30" s="54"/>
-      <c r="L30" s="44"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45"/>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="45"/>
-      <c r="R30" s="45"/>
-      <c r="S30" s="45"/>
-      <c r="T30" s="45"/>
-      <c r="U30" s="45"/>
-      <c r="V30" s="46"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="50"/>
+      <c r="V30" s="51"/>
       <c r="W30" s="23"/>
       <c r="AB30" s="13"/>
     </row>
     <row r="31" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A31" s="47" t="str">
+      <c r="A31" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="B31" s="48"/>
+      <c r="B31" s="41"/>
       <c r="C31" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D31" s="49"/>
-      <c r="E31" s="50"/>
-      <c r="F31" s="49"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="49"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="53" t="str">
+      <c r="D31" s="36"/>
+      <c r="E31" s="37"/>
+      <c r="F31" s="36"/>
+      <c r="G31" s="37"/>
+      <c r="H31" s="36"/>
+      <c r="I31" s="37"/>
+      <c r="J31" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K31" s="54"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45"/>
-      <c r="P31" s="45"/>
-      <c r="Q31" s="45"/>
-      <c r="R31" s="45"/>
-      <c r="S31" s="45"/>
-      <c r="T31" s="45"/>
-      <c r="U31" s="45"/>
-      <c r="V31" s="46"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="49"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="50"/>
+      <c r="O31" s="50"/>
+      <c r="P31" s="50"/>
+      <c r="Q31" s="50"/>
+      <c r="R31" s="50"/>
+      <c r="S31" s="50"/>
+      <c r="T31" s="50"/>
+      <c r="U31" s="50"/>
+      <c r="V31" s="51"/>
       <c r="W31" s="23"/>
       <c r="AB31" s="13"/>
     </row>
     <row r="32" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A32" s="47" t="str">
+      <c r="A32" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="B32" s="48"/>
+      <c r="B32" s="41"/>
       <c r="C32" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D32" s="49"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="49"/>
-      <c r="G32" s="50"/>
-      <c r="H32" s="49"/>
-      <c r="I32" s="50"/>
-      <c r="J32" s="53" t="str">
+      <c r="D32" s="36"/>
+      <c r="E32" s="37"/>
+      <c r="F32" s="36"/>
+      <c r="G32" s="37"/>
+      <c r="H32" s="36"/>
+      <c r="I32" s="37"/>
+      <c r="J32" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K32" s="54"/>
-      <c r="L32" s="44"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="45"/>
-      <c r="Q32" s="45"/>
-      <c r="R32" s="45"/>
-      <c r="S32" s="45"/>
-      <c r="T32" s="45"/>
-      <c r="U32" s="45"/>
-      <c r="V32" s="46"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="50"/>
+      <c r="P32" s="50"/>
+      <c r="Q32" s="50"/>
+      <c r="R32" s="50"/>
+      <c r="S32" s="50"/>
+      <c r="T32" s="50"/>
+      <c r="U32" s="50"/>
+      <c r="V32" s="51"/>
       <c r="W32" s="23"/>
       <c r="AB32" s="13"/>
     </row>
     <row r="33" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A33" s="47" t="str">
+      <c r="A33" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="B33" s="48"/>
+      <c r="B33" s="41"/>
       <c r="C33" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D33" s="49"/>
-      <c r="E33" s="50"/>
-      <c r="F33" s="49"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="49"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="53" t="str">
+      <c r="D33" s="36"/>
+      <c r="E33" s="37"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="37"/>
+      <c r="J33" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K33" s="54"/>
-      <c r="L33" s="44"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="45"/>
-      <c r="P33" s="45"/>
-      <c r="Q33" s="45"/>
-      <c r="R33" s="45"/>
-      <c r="S33" s="45"/>
-      <c r="T33" s="45"/>
-      <c r="U33" s="45"/>
-      <c r="V33" s="46"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="50"/>
+      <c r="N33" s="50"/>
+      <c r="O33" s="50"/>
+      <c r="P33" s="50"/>
+      <c r="Q33" s="50"/>
+      <c r="R33" s="50"/>
+      <c r="S33" s="50"/>
+      <c r="T33" s="50"/>
+      <c r="U33" s="50"/>
+      <c r="V33" s="51"/>
       <c r="W33" s="23"/>
       <c r="AB33" s="13"/>
     </row>
     <row r="34" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A34" s="47" t="str">
+      <c r="A34" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="B34" s="48"/>
+      <c r="B34" s="41"/>
       <c r="C34" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D34" s="51"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="50"/>
-      <c r="H34" s="49"/>
-      <c r="I34" s="50"/>
-      <c r="J34" s="53" t="str">
+      <c r="D34" s="42"/>
+      <c r="E34" s="43"/>
+      <c r="F34" s="36"/>
+      <c r="G34" s="37"/>
+      <c r="H34" s="36"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K34" s="54"/>
-      <c r="L34" s="44"/>
-      <c r="M34" s="45"/>
-      <c r="N34" s="45"/>
-      <c r="O34" s="45"/>
-      <c r="P34" s="45"/>
-      <c r="Q34" s="45"/>
-      <c r="R34" s="45"/>
-      <c r="S34" s="45"/>
-      <c r="T34" s="45"/>
-      <c r="U34" s="45"/>
-      <c r="V34" s="46"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="50"/>
+      <c r="N34" s="50"/>
+      <c r="O34" s="50"/>
+      <c r="P34" s="50"/>
+      <c r="Q34" s="50"/>
+      <c r="R34" s="50"/>
+      <c r="S34" s="50"/>
+      <c r="T34" s="50"/>
+      <c r="U34" s="50"/>
+      <c r="V34" s="51"/>
       <c r="W34" s="23"/>
       <c r="AB34" s="13"/>
     </row>
     <row r="35" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A35" s="47" t="str">
+      <c r="A35" s="40" t="str">
         <f t="shared" ca="1" si="4"/>
         <v/>
       </c>
-      <c r="B35" s="48"/>
+      <c r="B35" s="41"/>
       <c r="C35" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D35" s="51"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="49"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="49"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="53" t="str">
+      <c r="D35" s="42"/>
+      <c r="E35" s="43"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="37"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="37"/>
+      <c r="J35" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K35" s="54"/>
-      <c r="L35" s="44"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="45"/>
-      <c r="O35" s="45"/>
-      <c r="P35" s="45"/>
-      <c r="Q35" s="45"/>
-      <c r="R35" s="45"/>
-      <c r="S35" s="45"/>
-      <c r="T35" s="45"/>
-      <c r="U35" s="45"/>
-      <c r="V35" s="46"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="50"/>
+      <c r="N35" s="50"/>
+      <c r="O35" s="50"/>
+      <c r="P35" s="50"/>
+      <c r="Q35" s="50"/>
+      <c r="R35" s="50"/>
+      <c r="S35" s="50"/>
+      <c r="T35" s="50"/>
+      <c r="U35" s="50"/>
+      <c r="V35" s="51"/>
       <c r="W35" s="23"/>
       <c r="AB35" s="13"/>
     </row>
     <row r="36" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A36" s="47" t="str">
+      <c r="A36" s="40" t="str">
         <f t="shared" ref="A36:A44" ca="1" si="5">IF(A35="","",
 IF(OR(DAY(A35+1)&lt;=20, MONTH($A$14)=MONTH(A35+1)),A35+1,""))</f>
         <v/>
       </c>
-      <c r="B36" s="48"/>
+      <c r="B36" s="41"/>
       <c r="C36" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D36" s="51"/>
-      <c r="E36" s="52"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="53" t="str">
+      <c r="D36" s="42"/>
+      <c r="E36" s="43"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="37"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="37"/>
+      <c r="J36" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K36" s="54"/>
-      <c r="L36" s="44"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="45"/>
-      <c r="R36" s="45"/>
-      <c r="S36" s="45"/>
-      <c r="T36" s="45"/>
-      <c r="U36" s="45"/>
-      <c r="V36" s="46"/>
+      <c r="K36" s="39"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="50"/>
+      <c r="P36" s="50"/>
+      <c r="Q36" s="50"/>
+      <c r="R36" s="50"/>
+      <c r="S36" s="50"/>
+      <c r="T36" s="50"/>
+      <c r="U36" s="50"/>
+      <c r="V36" s="51"/>
       <c r="W36" s="23"/>
       <c r="AB36" s="13"/>
     </row>
     <row r="37" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A37" s="47" t="str">
+      <c r="A37" s="40" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="B37" s="48"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D37" s="51"/>
-      <c r="E37" s="52"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="53" t="str">
+      <c r="D37" s="42"/>
+      <c r="E37" s="43"/>
+      <c r="F37" s="36"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="36"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K37" s="54"/>
-      <c r="L37" s="44"/>
-      <c r="M37" s="45"/>
-      <c r="N37" s="45"/>
-      <c r="O37" s="45"/>
-      <c r="P37" s="45"/>
-      <c r="Q37" s="45"/>
-      <c r="R37" s="45"/>
-      <c r="S37" s="45"/>
-      <c r="T37" s="45"/>
-      <c r="U37" s="45"/>
-      <c r="V37" s="46"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="49"/>
+      <c r="M37" s="50"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="50"/>
+      <c r="P37" s="50"/>
+      <c r="Q37" s="50"/>
+      <c r="R37" s="50"/>
+      <c r="S37" s="50"/>
+      <c r="T37" s="50"/>
+      <c r="U37" s="50"/>
+      <c r="V37" s="51"/>
       <c r="W37" s="23"/>
       <c r="AB37" s="13"/>
     </row>
     <row r="38" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A38" s="47" t="str">
+      <c r="A38" s="40" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="B38" s="48"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D38" s="49"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="50"/>
-      <c r="H38" s="49"/>
-      <c r="I38" s="50"/>
-      <c r="J38" s="53" t="str">
+      <c r="D38" s="36"/>
+      <c r="E38" s="37"/>
+      <c r="F38" s="36"/>
+      <c r="G38" s="37"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="37"/>
+      <c r="J38" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K38" s="54"/>
-      <c r="L38" s="44"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="45"/>
-      <c r="O38" s="45"/>
-      <c r="P38" s="45"/>
-      <c r="Q38" s="45"/>
-      <c r="R38" s="45"/>
-      <c r="S38" s="45"/>
-      <c r="T38" s="45"/>
-      <c r="U38" s="45"/>
-      <c r="V38" s="46"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="50"/>
+      <c r="P38" s="50"/>
+      <c r="Q38" s="50"/>
+      <c r="R38" s="50"/>
+      <c r="S38" s="50"/>
+      <c r="T38" s="50"/>
+      <c r="U38" s="50"/>
+      <c r="V38" s="51"/>
       <c r="W38" s="23"/>
       <c r="AB38" s="13"/>
     </row>
     <row r="39" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A39" s="47" t="str">
+      <c r="A39" s="40" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="B39" s="48"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D39" s="49"/>
-      <c r="E39" s="50"/>
-      <c r="F39" s="49"/>
-      <c r="G39" s="50"/>
-      <c r="H39" s="49"/>
-      <c r="I39" s="50"/>
-      <c r="J39" s="53" t="str">
+      <c r="D39" s="36"/>
+      <c r="E39" s="37"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K39" s="54"/>
-      <c r="L39" s="44"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="45"/>
-      <c r="P39" s="45"/>
-      <c r="Q39" s="45"/>
-      <c r="R39" s="45"/>
-      <c r="S39" s="45"/>
-      <c r="T39" s="45"/>
-      <c r="U39" s="45"/>
-      <c r="V39" s="46"/>
+      <c r="K39" s="39"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="50"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="50"/>
+      <c r="P39" s="50"/>
+      <c r="Q39" s="50"/>
+      <c r="R39" s="50"/>
+      <c r="S39" s="50"/>
+      <c r="T39" s="50"/>
+      <c r="U39" s="50"/>
+      <c r="V39" s="51"/>
       <c r="W39" s="23"/>
       <c r="AB39" s="13"/>
     </row>
     <row r="40" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A40" s="47" t="str">
+      <c r="A40" s="40" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="B40" s="48"/>
+      <c r="B40" s="41"/>
       <c r="C40" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D40" s="51"/>
-      <c r="E40" s="52"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="50"/>
-      <c r="H40" s="49"/>
-      <c r="I40" s="50"/>
-      <c r="J40" s="53" t="str">
+      <c r="D40" s="42"/>
+      <c r="E40" s="43"/>
+      <c r="F40" s="36"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="36"/>
+      <c r="I40" s="37"/>
+      <c r="J40" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K40" s="54"/>
-      <c r="L40" s="44"/>
-      <c r="M40" s="45"/>
-      <c r="N40" s="45"/>
-      <c r="O40" s="45"/>
-      <c r="P40" s="45"/>
-      <c r="Q40" s="45"/>
-      <c r="R40" s="45"/>
-      <c r="S40" s="45"/>
-      <c r="T40" s="45"/>
-      <c r="U40" s="45"/>
-      <c r="V40" s="46"/>
+      <c r="K40" s="39"/>
+      <c r="L40" s="49"/>
+      <c r="M40" s="50"/>
+      <c r="N40" s="50"/>
+      <c r="O40" s="50"/>
+      <c r="P40" s="50"/>
+      <c r="Q40" s="50"/>
+      <c r="R40" s="50"/>
+      <c r="S40" s="50"/>
+      <c r="T40" s="50"/>
+      <c r="U40" s="50"/>
+      <c r="V40" s="51"/>
       <c r="W40" s="23"/>
       <c r="AB40" s="13"/>
     </row>
     <row r="41" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A41" s="47" t="str">
+      <c r="A41" s="40" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="B41" s="48"/>
+      <c r="B41" s="41"/>
       <c r="C41" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D41" s="51"/>
-      <c r="E41" s="52"/>
-      <c r="F41" s="49"/>
-      <c r="G41" s="50"/>
-      <c r="H41" s="49"/>
-      <c r="I41" s="50"/>
-      <c r="J41" s="53" t="str">
+      <c r="D41" s="42"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="36"/>
+      <c r="I41" s="37"/>
+      <c r="J41" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K41" s="54"/>
-      <c r="L41" s="44"/>
-      <c r="M41" s="45"/>
-      <c r="N41" s="45"/>
-      <c r="O41" s="45"/>
-      <c r="P41" s="45"/>
-      <c r="Q41" s="45"/>
-      <c r="R41" s="45"/>
-      <c r="S41" s="45"/>
-      <c r="T41" s="45"/>
-      <c r="U41" s="45"/>
-      <c r="V41" s="46"/>
+      <c r="K41" s="39"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="50"/>
+      <c r="N41" s="50"/>
+      <c r="O41" s="50"/>
+      <c r="P41" s="50"/>
+      <c r="Q41" s="50"/>
+      <c r="R41" s="50"/>
+      <c r="S41" s="50"/>
+      <c r="T41" s="50"/>
+      <c r="U41" s="50"/>
+      <c r="V41" s="51"/>
       <c r="W41" s="23"/>
       <c r="AB41" s="13"/>
     </row>
     <row r="42" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A42" s="47" t="str">
+      <c r="A42" s="40" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="41"/>
       <c r="C42" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D42" s="51"/>
-      <c r="E42" s="52"/>
-      <c r="F42" s="49"/>
-      <c r="G42" s="50"/>
-      <c r="H42" s="49"/>
-      <c r="I42" s="50"/>
-      <c r="J42" s="53" t="str">
+      <c r="D42" s="42"/>
+      <c r="E42" s="43"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="36"/>
+      <c r="I42" s="37"/>
+      <c r="J42" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K42" s="54"/>
-      <c r="L42" s="44"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="45"/>
-      <c r="R42" s="45"/>
-      <c r="S42" s="45"/>
-      <c r="T42" s="45"/>
-      <c r="U42" s="45"/>
-      <c r="V42" s="46"/>
+      <c r="K42" s="39"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="50"/>
+      <c r="N42" s="50"/>
+      <c r="O42" s="50"/>
+      <c r="P42" s="50"/>
+      <c r="Q42" s="50"/>
+      <c r="R42" s="50"/>
+      <c r="S42" s="50"/>
+      <c r="T42" s="50"/>
+      <c r="U42" s="50"/>
+      <c r="V42" s="51"/>
       <c r="W42" s="23"/>
       <c r="AB42" s="13"/>
     </row>
     <row r="43" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A43" s="47" t="str">
+      <c r="A43" s="40" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="B43" s="48"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D43" s="51"/>
-      <c r="E43" s="52"/>
-      <c r="F43" s="49"/>
-      <c r="G43" s="50"/>
-      <c r="H43" s="49"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="53" t="str">
+      <c r="D43" s="42"/>
+      <c r="E43" s="43"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="36"/>
+      <c r="I43" s="37"/>
+      <c r="J43" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K43" s="54"/>
-      <c r="L43" s="44"/>
-      <c r="M43" s="45"/>
-      <c r="N43" s="45"/>
-      <c r="O43" s="45"/>
-      <c r="P43" s="45"/>
-      <c r="Q43" s="45"/>
-      <c r="R43" s="45"/>
-      <c r="S43" s="45"/>
-      <c r="T43" s="45"/>
-      <c r="U43" s="45"/>
-      <c r="V43" s="46"/>
+      <c r="K43" s="39"/>
+      <c r="L43" s="49"/>
+      <c r="M43" s="50"/>
+      <c r="N43" s="50"/>
+      <c r="O43" s="50"/>
+      <c r="P43" s="50"/>
+      <c r="Q43" s="50"/>
+      <c r="R43" s="50"/>
+      <c r="S43" s="50"/>
+      <c r="T43" s="50"/>
+      <c r="U43" s="50"/>
+      <c r="V43" s="51"/>
       <c r="W43" s="23"/>
       <c r="AB43" s="13"/>
     </row>
     <row r="44" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A44" s="47" t="str">
+      <c r="A44" s="40" t="str">
         <f t="shared" ca="1" si="5"/>
         <v/>
       </c>
-      <c r="B44" s="48"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v/>
       </c>
-      <c r="D44" s="49"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="49"/>
-      <c r="G44" s="50"/>
-      <c r="H44" s="49"/>
-      <c r="I44" s="50"/>
-      <c r="J44" s="53" t="str">
+      <c r="D44" s="36"/>
+      <c r="E44" s="37"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="36"/>
+      <c r="I44" s="37"/>
+      <c r="J44" s="38" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="K44" s="54"/>
-      <c r="L44" s="44"/>
-      <c r="M44" s="45"/>
-      <c r="N44" s="45"/>
-      <c r="O44" s="45"/>
-      <c r="P44" s="45"/>
-      <c r="Q44" s="45"/>
-      <c r="R44" s="45"/>
-      <c r="S44" s="45"/>
-      <c r="T44" s="45"/>
-      <c r="U44" s="45"/>
-      <c r="V44" s="46"/>
+      <c r="K44" s="39"/>
+      <c r="L44" s="49"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="50"/>
+      <c r="P44" s="50"/>
+      <c r="Q44" s="50"/>
+      <c r="R44" s="50"/>
+      <c r="S44" s="50"/>
+      <c r="T44" s="50"/>
+      <c r="U44" s="50"/>
+      <c r="V44" s="51"/>
       <c r="W44" s="23"/>
       <c r="AB44" s="13"/>
     </row>
@@ -20522,241 +20479,232 @@
       <c r="T45" s="22"/>
       <c r="U45" s="22"/>
       <c r="V45" s="22"/>
-      <c r="W45" s="22"/>
-      <c r="X45" s="22"/>
-      <c r="Y45" s="22"/>
+      <c r="W45" s="131"/>
+      <c r="X45" s="131"/>
+      <c r="Y45" s="131"/>
       <c r="Z45" s="22"/>
       <c r="AA45" s="19"/>
     </row>
     <row r="46" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A46" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" s="42"/>
-      <c r="C46" s="42"/>
-      <c r="D46" s="42"/>
-      <c r="E46" s="42"/>
-      <c r="F46" s="42"/>
-      <c r="G46" s="42"/>
-      <c r="H46" s="42"/>
-      <c r="I46" s="42"/>
-      <c r="J46" s="42"/>
-      <c r="K46" s="42"/>
-      <c r="L46" s="42"/>
-      <c r="M46" s="42"/>
-      <c r="N46" s="42"/>
-      <c r="O46" s="42"/>
-      <c r="P46" s="42"/>
-      <c r="Q46" s="42"/>
-      <c r="R46" s="42"/>
-      <c r="S46" s="42"/>
-      <c r="T46" s="42"/>
-      <c r="U46" s="42"/>
-      <c r="V46" s="42"/>
-      <c r="W46" s="42"/>
-      <c r="X46" s="42"/>
-      <c r="Y46" s="43"/>
+      <c r="A46" s="121" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="122"/>
+      <c r="C46" s="122"/>
+      <c r="D46" s="122"/>
+      <c r="E46" s="122"/>
+      <c r="F46" s="122"/>
+      <c r="G46" s="122"/>
+      <c r="H46" s="122"/>
+      <c r="I46" s="122"/>
+      <c r="J46" s="122"/>
+      <c r="K46" s="122"/>
+      <c r="L46" s="122"/>
+      <c r="M46" s="122"/>
+      <c r="N46" s="122"/>
+      <c r="O46" s="122"/>
+      <c r="P46" s="122"/>
+      <c r="Q46" s="122"/>
+      <c r="R46" s="122"/>
+      <c r="S46" s="122"/>
+      <c r="T46" s="122"/>
+      <c r="U46" s="122"/>
+      <c r="V46" s="123"/>
+      <c r="W46" s="131"/>
+      <c r="X46" s="131"/>
+      <c r="Y46" s="131"/>
       <c r="Z46" s="22"/>
       <c r="AA46" s="19"/>
     </row>
     <row r="47" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A47" s="35"/>
-      <c r="B47" s="36"/>
-      <c r="C47" s="36"/>
-      <c r="D47" s="36"/>
-      <c r="E47" s="36"/>
-      <c r="F47" s="36"/>
-      <c r="G47" s="36"/>
-      <c r="H47" s="36"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
-      <c r="K47" s="36"/>
-      <c r="L47" s="36"/>
-      <c r="M47" s="36"/>
-      <c r="N47" s="36"/>
-      <c r="O47" s="36"/>
-      <c r="P47" s="36"/>
-      <c r="Q47" s="36"/>
-      <c r="R47" s="36"/>
-      <c r="S47" s="36"/>
-      <c r="T47" s="36"/>
-      <c r="U47" s="36"/>
-      <c r="V47" s="36"/>
-      <c r="W47" s="36"/>
-      <c r="X47" s="36"/>
-      <c r="Y47" s="37"/>
+      <c r="A47" s="127"/>
+      <c r="B47" s="128"/>
+      <c r="C47" s="128"/>
+      <c r="D47" s="128"/>
+      <c r="E47" s="128"/>
+      <c r="F47" s="128"/>
+      <c r="G47" s="128"/>
+      <c r="H47" s="128"/>
+      <c r="I47" s="128"/>
+      <c r="J47" s="128"/>
+      <c r="K47" s="128"/>
+      <c r="L47" s="128"/>
+      <c r="M47" s="128"/>
+      <c r="N47" s="128"/>
+      <c r="O47" s="128"/>
+      <c r="P47" s="128"/>
+      <c r="Q47" s="128"/>
+      <c r="R47" s="128"/>
+      <c r="S47" s="128"/>
+      <c r="T47" s="128"/>
+      <c r="U47" s="128"/>
+      <c r="V47" s="134"/>
+      <c r="W47" s="132"/>
+      <c r="X47" s="132"/>
+      <c r="Y47" s="132"/>
       <c r="Z47" s="22"/>
       <c r="AA47" s="19"/>
     </row>
     <row r="48" spans="1:28" ht="23.1" customHeight="1">
-      <c r="A48" s="35"/>
-      <c r="B48" s="36"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="36"/>
-      <c r="F48" s="36"/>
-      <c r="G48" s="36"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="36"/>
-      <c r="J48" s="36"/>
-      <c r="K48" s="36"/>
-      <c r="L48" s="36"/>
-      <c r="M48" s="36"/>
-      <c r="N48" s="36"/>
-      <c r="O48" s="36"/>
-      <c r="P48" s="36"/>
-      <c r="Q48" s="36"/>
-      <c r="R48" s="36"/>
-      <c r="S48" s="36"/>
-      <c r="T48" s="36"/>
-      <c r="U48" s="36"/>
-      <c r="V48" s="36"/>
-      <c r="W48" s="36"/>
-      <c r="X48" s="36"/>
-      <c r="Y48" s="37"/>
+      <c r="A48" s="127"/>
+      <c r="B48" s="128"/>
+      <c r="C48" s="128"/>
+      <c r="D48" s="128"/>
+      <c r="E48" s="128"/>
+      <c r="F48" s="128"/>
+      <c r="G48" s="128"/>
+      <c r="H48" s="128"/>
+      <c r="I48" s="128"/>
+      <c r="J48" s="128"/>
+      <c r="K48" s="128"/>
+      <c r="L48" s="128"/>
+      <c r="M48" s="128"/>
+      <c r="N48" s="128"/>
+      <c r="O48" s="128"/>
+      <c r="P48" s="128"/>
+      <c r="Q48" s="128"/>
+      <c r="R48" s="128"/>
+      <c r="S48" s="128"/>
+      <c r="T48" s="128"/>
+      <c r="U48" s="128"/>
+      <c r="V48" s="134"/>
+      <c r="W48" s="132"/>
+      <c r="X48" s="132"/>
+      <c r="Y48" s="132"/>
       <c r="Z48" s="22"/>
       <c r="AA48" s="19"/>
     </row>
     <row r="49" spans="1:27" ht="23.1" customHeight="1">
-      <c r="A49" s="38"/>
-      <c r="B49" s="39"/>
-      <c r="C49" s="39"/>
-      <c r="D49" s="39"/>
-      <c r="E49" s="39"/>
-      <c r="F49" s="39"/>
-      <c r="G49" s="39"/>
-      <c r="H49" s="39"/>
-      <c r="I49" s="39"/>
-      <c r="J49" s="39"/>
-      <c r="K49" s="39"/>
-      <c r="L49" s="39"/>
-      <c r="M49" s="39"/>
-      <c r="N49" s="39"/>
-      <c r="O49" s="39"/>
-      <c r="P49" s="39"/>
-      <c r="Q49" s="39"/>
-      <c r="R49" s="39"/>
-      <c r="S49" s="39"/>
-      <c r="T49" s="39"/>
-      <c r="U49" s="39"/>
-      <c r="V49" s="39"/>
-      <c r="W49" s="39"/>
-      <c r="X49" s="39"/>
-      <c r="Y49" s="40"/>
+      <c r="A49" s="129"/>
+      <c r="B49" s="130"/>
+      <c r="C49" s="130"/>
+      <c r="D49" s="130"/>
+      <c r="E49" s="130"/>
+      <c r="F49" s="130"/>
+      <c r="G49" s="130"/>
+      <c r="H49" s="130"/>
+      <c r="I49" s="130"/>
+      <c r="J49" s="130"/>
+      <c r="K49" s="130"/>
+      <c r="L49" s="130"/>
+      <c r="M49" s="130"/>
+      <c r="N49" s="130"/>
+      <c r="O49" s="130"/>
+      <c r="P49" s="130"/>
+      <c r="Q49" s="130"/>
+      <c r="R49" s="130"/>
+      <c r="S49" s="130"/>
+      <c r="T49" s="130"/>
+      <c r="U49" s="130"/>
+      <c r="V49" s="135"/>
+      <c r="W49" s="132"/>
+      <c r="X49" s="132"/>
+      <c r="Y49" s="132"/>
       <c r="Z49" s="22"/>
       <c r="AA49" s="19"/>
     </row>
+    <row r="50" spans="1:27" ht="15" customHeight="1">
+      <c r="W50" s="133"/>
+      <c r="X50" s="133"/>
+      <c r="Y50" s="133"/>
+    </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="227">
-    <mergeCell ref="H27:I27"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="J26:K26"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="H24:I24"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="J24:K24"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="J22:K22"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="L20:V20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="H15:I15"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="L19:V19"/>
-    <mergeCell ref="L18:V18"/>
-    <mergeCell ref="L17:V17"/>
-    <mergeCell ref="L16:V16"/>
-    <mergeCell ref="L15:V15"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="L11:V12"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:G7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:G8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="E9:G9"/>
-    <mergeCell ref="A11:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="L13:V13"/>
-    <mergeCell ref="L14:V14"/>
-    <mergeCell ref="D11:E12"/>
-    <mergeCell ref="F11:G12"/>
-    <mergeCell ref="H11:I12"/>
-    <mergeCell ref="J11:K12"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="V4:W4"/>
-    <mergeCell ref="X4:Y4"/>
-    <mergeCell ref="V5:W7"/>
-    <mergeCell ref="X5:Y7"/>
-    <mergeCell ref="A1:J2"/>
-    <mergeCell ref="Q1:R2"/>
-    <mergeCell ref="S1:Y2"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:G4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="R4:T5"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="O4:Q5"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:G5"/>
-    <mergeCell ref="I7:K7"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="L35:V35"/>
-    <mergeCell ref="L36:V36"/>
-    <mergeCell ref="L37:V37"/>
-    <mergeCell ref="L38:V38"/>
-    <mergeCell ref="L39:V39"/>
-    <mergeCell ref="L21:V21"/>
-    <mergeCell ref="L22:V22"/>
-    <mergeCell ref="L23:V23"/>
-    <mergeCell ref="L24:V24"/>
-    <mergeCell ref="L25:V25"/>
-    <mergeCell ref="L26:V26"/>
-    <mergeCell ref="L27:V27"/>
-    <mergeCell ref="L28:V28"/>
-    <mergeCell ref="L29:V29"/>
-    <mergeCell ref="L32:V32"/>
-    <mergeCell ref="L31:V31"/>
-    <mergeCell ref="L30:V30"/>
+  <mergeCells count="225">
+    <mergeCell ref="A47:V49"/>
+    <mergeCell ref="A46:V46"/>
+    <mergeCell ref="L44:V44"/>
+    <mergeCell ref="L43:V43"/>
+    <mergeCell ref="L42:V42"/>
+    <mergeCell ref="L41:V41"/>
+    <mergeCell ref="L40:V40"/>
+    <mergeCell ref="L34:V34"/>
+    <mergeCell ref="L33:V33"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="J42:K42"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="J44:K44"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F27:G27"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="J30:K30"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="H29:I29"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="H28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F31:G31"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="H30:I30"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="J33:K33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="J34:K34"/>
+    <mergeCell ref="J35:K35"/>
+    <mergeCell ref="F33:G33"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="H35:I35"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A39:B39"/>
     <mergeCell ref="A40:B40"/>
@@ -20781,101 +20729,113 @@
     <mergeCell ref="H36:I36"/>
     <mergeCell ref="H37:I37"/>
     <mergeCell ref="H38:I38"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="J33:K33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="J34:K34"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="F33:G33"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F35:G35"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="H30:I30"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="H29:I29"/>
-    <mergeCell ref="J29:K29"/>
-    <mergeCell ref="H28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F27:G27"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="L35:V35"/>
+    <mergeCell ref="L36:V36"/>
+    <mergeCell ref="L37:V37"/>
+    <mergeCell ref="L38:V38"/>
+    <mergeCell ref="L39:V39"/>
+    <mergeCell ref="L21:V21"/>
+    <mergeCell ref="L22:V22"/>
+    <mergeCell ref="L23:V23"/>
+    <mergeCell ref="L24:V24"/>
+    <mergeCell ref="L25:V25"/>
+    <mergeCell ref="L26:V26"/>
+    <mergeCell ref="L27:V27"/>
+    <mergeCell ref="L28:V28"/>
+    <mergeCell ref="L29:V29"/>
+    <mergeCell ref="L32:V32"/>
+    <mergeCell ref="L31:V31"/>
+    <mergeCell ref="L30:V30"/>
+    <mergeCell ref="A1:J2"/>
+    <mergeCell ref="Q1:R2"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="I4:K4"/>
+    <mergeCell ref="R4:T5"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="O4:Q5"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="S1:V2"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="X4:Y4"/>
+    <mergeCell ref="X5:Y7"/>
+    <mergeCell ref="I7:K7"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="L13:V13"/>
+    <mergeCell ref="L14:V14"/>
+    <mergeCell ref="D11:E12"/>
+    <mergeCell ref="F11:G12"/>
+    <mergeCell ref="H11:I12"/>
+    <mergeCell ref="J11:K12"/>
+    <mergeCell ref="I6:K6"/>
+    <mergeCell ref="L11:V12"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="A11:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="J13:K13"/>
+    <mergeCell ref="L20:V20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="L19:V19"/>
+    <mergeCell ref="L18:V18"/>
+    <mergeCell ref="L17:V17"/>
+    <mergeCell ref="L16:V16"/>
+    <mergeCell ref="L15:V15"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="J23:K23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="J24:K24"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="J27:K27"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="J26:K26"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="H24:I24"/>
     <mergeCell ref="F26:G26"/>
-    <mergeCell ref="A47:Y49"/>
-    <mergeCell ref="A46:Y46"/>
-    <mergeCell ref="L44:V44"/>
-    <mergeCell ref="L43:V43"/>
-    <mergeCell ref="L42:V42"/>
-    <mergeCell ref="L41:V41"/>
-    <mergeCell ref="L40:V40"/>
-    <mergeCell ref="L34:V34"/>
-    <mergeCell ref="L33:V33"/>
-    <mergeCell ref="J43:K43"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="J42:K42"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="J44:K44"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="H43:I43"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <conditionalFormatting sqref="A1:J2 E8:G9">
@@ -20896,7 +20856,7 @@
       <formula>#REF!="振替稼働"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="S1:Y2">
+  <conditionalFormatting sqref="S1 W1:Y2">
     <cfRule type="containsText" dxfId="0" priority="9" operator="containsText" text="入力してください">
       <formula>NOT(ISERROR(SEARCH("入力してください",S1)))</formula>
     </cfRule>
@@ -20905,12 +20865,11 @@
     <dataValidation type="decimal" imeMode="off" operator="greaterThanOrEqual" allowBlank="1" showDropDown="1" showInputMessage="1" showErrorMessage="1" error="半角で時刻を入力してください　例)10:00" sqref="E4:G6 D13:K44" xr:uid="{47CC238B-533E-4FBF-891A-2E863C4F6A4B}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation imeMode="hiragana" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S1:Y2 A47:Y49 L14:V44" xr:uid="{52D4DF7A-1DCB-45EB-9020-1B299194C4C6}"/>
+    <dataValidation imeMode="hiragana" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L14:V44 S1 W1:Y2 W47:Y49 A47" xr:uid="{52D4DF7A-1DCB-45EB-9020-1B299194C4C6}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="69" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" scale="71" pageOrder="overThenDown" orientation="portrait" cellComments="atEnd" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>